<commit_message>
Posted SRM 155 Div 2
</commit_message>
<xml_diff>
--- a/TCS_Notes.xlsx
+++ b/TCS_Notes.xlsx
@@ -767,7 +767,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,7 +1530,7 @@
         <v>39</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>

</xml_diff>

<commit_message>
Finished SRM 156 DIV 2.  Not posted.
</commit_message>
<xml_diff>
--- a/TCS_Notes.xlsx
+++ b/TCS_Notes.xlsx
@@ -779,11 +779,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,1162 +843,1236 @@
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>155</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="12">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>156</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12">
         <v>250</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
-        <v>155</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16">
-        <v>500</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>155</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>8</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16">
-        <v>1000</v>
-      </c>
-      <c r="G10" s="16">
-        <v>300</v>
-      </c>
+      <c r="E10" s="16">
+        <v>600</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
-        <v>155</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>74</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="F11" s="16">
+        <v>1000</v>
+      </c>
       <c r="G11" s="16"/>
-      <c r="H11" s="16">
-        <v>450</v>
-      </c>
+      <c r="H11" s="16"/>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
+        <v>156</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>156</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>155</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>154</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="12">
-        <v>300</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>154</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16">
-        <v>450</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="17"/>
+      <c r="B14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="12">
+        <v>250</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16">
-        <v>1000</v>
-      </c>
+      <c r="E15" s="16">
+        <v>500</v>
+      </c>
+      <c r="F15" s="16"/>
       <c r="G15" s="16"/>
-      <c r="H15" s="16">
-        <v>500</v>
-      </c>
+      <c r="H15" s="16"/>
       <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="F16" s="16">
+        <v>1000</v>
+      </c>
       <c r="G16" s="16">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
+    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>155</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16">
+        <v>450</v>
+      </c>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>155</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
         <v>154</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>153</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="12" t="s">
+      <c r="B19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="12">
-        <v>250</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>153</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16">
-        <v>500</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16">
-        <v>250</v>
-      </c>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17"/>
+      <c r="D19" s="12">
+        <v>300</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16">
-        <v>1000</v>
-      </c>
+      <c r="E20" s="16">
+        <v>450</v>
+      </c>
+      <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
+      <c r="F21" s="16">
+        <v>1000</v>
+      </c>
       <c r="G21" s="16"/>
       <c r="H21" s="16">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>154</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16">
+        <v>350</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <v>154</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
         <v>153</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="20" t="s">
+      <c r="B24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>152</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="12">
+      <c r="D24" s="12">
         <v>250</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
-        <v>152</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16">
-        <v>500</v>
-      </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16">
-        <v>250</v>
-      </c>
-      <c r="H24" s="16"/>
-      <c r="I24" s="17"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="13"/>
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16">
-        <v>1000</v>
-      </c>
-      <c r="G25" s="16"/>
+      <c r="E25" s="16">
+        <v>500</v>
+      </c>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16">
+        <v>250</v>
+      </c>
       <c r="H25" s="16"/>
       <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
+      <c r="F26" s="16">
+        <v>1000</v>
+      </c>
       <c r="G26" s="16"/>
-      <c r="H26" s="16">
-        <v>500</v>
-      </c>
+      <c r="H26" s="16"/>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18">
+    <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>153</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16">
+        <v>450</v>
+      </c>
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
+        <v>153</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
         <v>152</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
-        <v>151</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="12" t="s">
+      <c r="B29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D29" s="12">
         <v>250</v>
       </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="13"/>
-    </row>
-    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
-        <v>151</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16">
-        <v>500</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="17"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="13"/>
     </row>
     <row r="30" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16">
-        <v>1000</v>
-      </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16">
+      <c r="E30" s="16">
         <v>500</v>
       </c>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16">
+        <v>250</v>
+      </c>
+      <c r="H30" s="16"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16">
-        <v>250</v>
-      </c>
+      <c r="F31" s="16">
+        <v>1000</v>
+      </c>
+      <c r="G31" s="16"/>
       <c r="H31" s="16"/>
       <c r="I31" s="17"/>
     </row>
-    <row r="32" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18">
+    <row r="32" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>152</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16">
+        <v>500</v>
+      </c>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <v>152</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
         <v>151</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
-        <v>150</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="12">
+      <c r="B34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="12">
         <v>250</v>
       </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="13"/>
-    </row>
-    <row r="34" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
-        <v>150</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16">
-        <v>500</v>
-      </c>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16">
-        <v>250</v>
-      </c>
-      <c r="H34" s="16"/>
-      <c r="I34" s="17"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16">
-        <v>1100</v>
-      </c>
+      <c r="E35" s="16">
+        <v>500</v>
+      </c>
+      <c r="F35" s="16"/>
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
       <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
+      <c r="F36" s="16">
+        <v>1000</v>
+      </c>
       <c r="G36" s="16"/>
       <c r="H36" s="16">
         <v>500</v>
       </c>
       <c r="I36" s="17"/>
     </row>
-    <row r="37" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18">
+    <row r="37" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>151</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16">
+        <v>250</v>
+      </c>
+      <c r="H37" s="16"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <v>151</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
         <v>150</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
-        <v>149</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="12">
+      <c r="B39" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="12">
         <v>250</v>
       </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="13"/>
-    </row>
-    <row r="39" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
-        <v>149</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16">
-        <v>500</v>
-      </c>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16">
-        <v>250</v>
-      </c>
-      <c r="H39" s="16"/>
-      <c r="I39" s="17"/>
-    </row>
-    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16">
-        <v>1000</v>
-      </c>
-      <c r="G40" s="16"/>
+      <c r="E40" s="16">
+        <v>500</v>
+      </c>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16">
+        <v>250</v>
+      </c>
       <c r="H40" s="16"/>
       <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
+      <c r="F41" s="16">
+        <v>1100</v>
+      </c>
       <c r="G41" s="16"/>
-      <c r="H41" s="16">
+      <c r="H41" s="16"/>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>150</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16">
         <v>500</v>
       </c>
-      <c r="I41" s="17"/>
-    </row>
-    <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18">
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18">
+        <v>150</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
         <v>149</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B44" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="12">
+        <v>250</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>149</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16">
+        <v>500</v>
+      </c>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16">
+        <v>250</v>
+      </c>
+      <c r="H45" s="16"/>
+      <c r="I45" s="17"/>
+    </row>
+    <row r="46" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>149</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16">
+        <v>1000</v>
+      </c>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>149</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16">
+        <v>500</v>
+      </c>
+      <c r="I47" s="17"/>
+    </row>
+    <row r="48" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18">
+        <v>149</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C48" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="21">
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="21">
         <v>1000</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="22">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="22">
         <v>148</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B49" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="24">
+      <c r="C49" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="24">
         <v>250</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="25"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="26">
-        <v>148</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8">
-        <v>600</v>
-      </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="27"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="26">
-        <v>148</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8">
-        <v>1000</v>
-      </c>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8">
-        <v>450</v>
-      </c>
-      <c r="I45" s="27"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="26">
-        <v>148</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8">
-        <v>250</v>
-      </c>
-      <c r="H46" s="8"/>
-      <c r="I46" s="27"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="28">
-        <v>148</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22">
-        <v>147</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="24">
-        <v>250</v>
-      </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="25"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="26">
-        <v>147</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8">
-        <v>600</v>
-      </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8">
-        <v>350</v>
-      </c>
-      <c r="H49" s="8"/>
-      <c r="I49" s="27"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="25"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="26">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8">
-        <v>950</v>
-      </c>
+      <c r="E50" s="8">
+        <v>600</v>
+      </c>
+      <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="27"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="26">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
+      <c r="F51" s="8">
+        <v>1000</v>
+      </c>
       <c r="G51" s="8"/>
       <c r="H51" s="8">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="I51" s="27"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="28">
+      <c r="A52" s="26">
+        <v>148</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8">
+        <v>250</v>
+      </c>
+      <c r="H52" s="8"/>
+      <c r="I52" s="27"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="28">
+        <v>148</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="30"/>
+      <c r="I53" s="31">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="22">
         <v>147</v>
       </c>
-      <c r="B52" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="30"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="31">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="32">
-        <v>146</v>
-      </c>
-      <c r="B53" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="24">
+      <c r="B54" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="24">
         <v>250</v>
       </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="25"/>
-    </row>
-    <row r="54" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="34">
-        <v>146</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8">
-        <v>500</v>
-      </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8">
-        <v>300</v>
-      </c>
-      <c r="H54" s="8"/>
-      <c r="I54" s="27"/>
-    </row>
-    <row r="55" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="34">
-        <v>146</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" s="8" t="s">
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="25"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="26">
+        <v>147</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8">
-        <v>1000</v>
-      </c>
-      <c r="G55" s="8"/>
+      <c r="E55" s="8">
+        <v>600</v>
+      </c>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8">
+        <v>350</v>
+      </c>
       <c r="H55" s="8"/>
       <c r="I55" s="27"/>
     </row>
-    <row r="56" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="34">
-        <v>146</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C56" s="8" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="26">
+        <v>147</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
+      <c r="F56" s="8">
+        <v>950</v>
+      </c>
       <c r="G56" s="8"/>
-      <c r="H56" s="8">
-        <v>600</v>
-      </c>
+      <c r="H56" s="8"/>
       <c r="I56" s="27"/>
     </row>
-    <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="26">
+        <v>147</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8">
+        <v>500</v>
+      </c>
+      <c r="I57" s="27"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="28">
+        <v>147</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="31">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="32">
         <v>146</v>
       </c>
-      <c r="B57" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="31">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="32">
-        <v>145</v>
-      </c>
-      <c r="B58" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="24">
+      <c r="B59" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="24">
         <v>250</v>
       </c>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="25"/>
-    </row>
-    <row r="59" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="34">
-        <v>145</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8">
-        <v>500</v>
-      </c>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="27"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="25"/>
     </row>
     <row r="60" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="34">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8">
-        <v>1100</v>
-      </c>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8">
-        <v>600</v>
-      </c>
+      <c r="E60" s="8">
+        <v>500</v>
+      </c>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8">
+        <v>300</v>
+      </c>
+      <c r="H60" s="8"/>
       <c r="I60" s="27"/>
     </row>
     <row r="61" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="34">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8">
-        <v>250</v>
-      </c>
+      <c r="F61" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G61" s="8"/>
       <c r="H61" s="8"/>
       <c r="I61" s="27"/>
     </row>
     <row r="62" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35">
+      <c r="A62" s="34">
+        <v>146</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8">
+        <v>600</v>
+      </c>
+      <c r="I62" s="27"/>
+    </row>
+    <row r="63" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="35">
+        <v>146</v>
+      </c>
+      <c r="B63" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="31">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="32">
         <v>145</v>
       </c>
-      <c r="B62" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C62" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="31">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="32">
-        <v>144</v>
-      </c>
-      <c r="B63" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="24">
-        <v>200</v>
-      </c>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="24"/>
-      <c r="H63" s="24"/>
-      <c r="I63" s="25"/>
-    </row>
-    <row r="64" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="34">
-        <v>144</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8">
-        <v>550</v>
-      </c>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8">
-        <v>300</v>
-      </c>
-      <c r="H64" s="8"/>
-      <c r="I64" s="27"/>
+      <c r="B64" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="24">
+        <v>250</v>
+      </c>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="24"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="25"/>
     </row>
     <row r="65" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="34">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8">
-        <v>1100</v>
-      </c>
+      <c r="E65" s="8">
+        <v>500</v>
+      </c>
+      <c r="F65" s="8"/>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
       <c r="I65" s="27"/>
     </row>
     <row r="66" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="34">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
+      <c r="F66" s="8">
+        <v>1100</v>
+      </c>
       <c r="G66" s="8"/>
       <c r="H66" s="8">
+        <v>600</v>
+      </c>
+      <c r="I66" s="27"/>
+    </row>
+    <row r="67" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="34">
+        <v>145</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8">
+        <v>250</v>
+      </c>
+      <c r="H67" s="8"/>
+      <c r="I67" s="27"/>
+    </row>
+    <row r="68" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="35">
+        <v>145</v>
+      </c>
+      <c r="B68" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="31">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="32">
+        <v>144</v>
+      </c>
+      <c r="B69" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="24">
+        <v>200</v>
+      </c>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="25"/>
+    </row>
+    <row r="70" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="34">
+        <v>144</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8">
         <v>550</v>
       </c>
-      <c r="I66" s="27"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="35">
+      <c r="F70" s="8"/>
+      <c r="G70" s="8">
+        <v>300</v>
+      </c>
+      <c r="H70" s="8"/>
+      <c r="I70" s="27"/>
+    </row>
+    <row r="71" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="34">
         <v>144</v>
       </c>
-      <c r="B67" s="36" t="s">
+      <c r="B71" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8">
+        <v>1100</v>
+      </c>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="27"/>
+    </row>
+    <row r="72" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="34">
+        <v>144</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8">
+        <v>550</v>
+      </c>
+      <c r="I72" s="27"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="35">
+        <v>144</v>
+      </c>
+      <c r="B73" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C67" s="30" t="s">
+      <c r="C73" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="30"/>
-      <c r="I67" s="31">
+      <c r="D73" s="30"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="30"/>
+      <c r="G73" s="30"/>
+      <c r="H73" s="30"/>
+      <c r="I73" s="31">
         <v>1100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Posted SRM 156 - DIV 2
</commit_message>
<xml_diff>
--- a/TCS_Notes.xlsx
+++ b/TCS_Notes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
   <si>
     <t>Match</t>
   </si>
@@ -253,6 +253,21 @@
   </si>
   <si>
     <t>RedBlack</t>
+  </si>
+  <si>
+    <t>DiskSpace</t>
+  </si>
+  <si>
+    <t>BombSweeper</t>
+  </si>
+  <si>
+    <t>WordParts</t>
+  </si>
+  <si>
+    <t>SmartElevator</t>
+  </si>
+  <si>
+    <t>PathFinding</t>
   </si>
 </sst>
 </file>
@@ -783,7 +798,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,8 +864,12 @@
       <c r="A9" s="10">
         <v>156</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="D9" s="12">
         <v>250</v>
       </c>
@@ -864,14 +883,20 @@
       <c r="A10" s="14">
         <v>156</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16">
         <v>600</v>
       </c>
       <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="G10" s="16">
+        <v>300</v>
+      </c>
       <c r="H10" s="16"/>
       <c r="I10" s="17"/>
     </row>
@@ -879,8 +904,12 @@
       <c r="A11" s="14">
         <v>156</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
+      <c r="B11" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16">
@@ -894,27 +923,35 @@
       <c r="A12" s="14">
         <v>156</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="H12" s="16">
+        <v>550</v>
+      </c>
       <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>156</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
-      <c r="I13" s="21"/>
+      <c r="I13" s="21">
+        <v>900</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">

</xml_diff>

<commit_message>
PickTeam working, not written up.
</commit_message>
<xml_diff>
--- a/TCS_Notes.xlsx
+++ b/TCS_Notes.xlsx
@@ -798,7 +798,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1191,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1229,7 +1229,7 @@
         <v>51</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>

</xml_diff>